<commit_message>
update many thing including FreqMesure, key and so on.
</commit_message>
<xml_diff>
--- a/Pin_list.xlsx
+++ b/Pin_list.xlsx
@@ -1,15 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\my_project\ELECAP\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{180555F9-439A-4282-A2A5-B4BAC0181EFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -18,14 +25,126 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+  <si>
+    <t>I2C1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PB6/SCL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PB7/SDA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FREQ1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PE5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FREQ2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PE6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UART1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA2/TX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA3/RX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DAC1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DAC2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CD4052</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A0/PE0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AE/PE1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SW/ACDC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PE2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SW/20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PE3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -53,7 +172,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +449,114 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>